<commit_message>
fix letter generation (C* was not in table)
changed recommendations
</commit_message>
<xml_diff>
--- a/elternbrief/ergebnisse.xlsx
+++ b/elternbrief/ergebnisse.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="49">
   <si>
     <t>Kategorie</t>
   </si>
@@ -158,6 +158,15 @@
   </si>
   <si>
     <t>Ihr Kind hat leider nicht teilgenommen.</t>
+  </si>
+  <si>
+    <t>3C*</t>
+  </si>
+  <si>
+    <t>4C*</t>
+  </si>
+  <si>
+    <t>5C*</t>
   </si>
 </sst>
 </file>
@@ -496,22 +505,22 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -828,10 +837,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="A1:D14"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,114 +936,156 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="37.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>37</v>
+      <c r="A7" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="37.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="37.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>39</v>
+      <c r="A9" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>21</v>
+        <v>15</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="37.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>24</v>
+        <v>18</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="37.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>41</v>
+      <c r="A11" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>24</v>
+        <v>18</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="37.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>24</v>
+        <v>20</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="37.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="37.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="37.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="37.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B16" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C16" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D16" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5">
+    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="5">
         <v>0</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B17" s="4">
         <v>0</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C17" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="7"/>
+      <c r="D17" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1047,7 +1098,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E16"/>
+      <selection activeCell="D11" sqref="D11:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1065,13 +1116,13 @@
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9"/>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="19" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="8"/>
@@ -1084,7 +1135,7 @@
       <c r="C3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="20" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="8"/>
@@ -1097,7 +1148,7 @@
       <c r="C4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="16"/>
+      <c r="D4" s="21"/>
       <c r="E4" s="8"/>
     </row>
     <row r="5" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -1108,7 +1159,7 @@
       <c r="C5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="16"/>
+      <c r="D5" s="21"/>
       <c r="E5" s="8"/>
     </row>
     <row r="6" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -1119,7 +1170,7 @@
       <c r="C6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="16"/>
+      <c r="D6" s="21"/>
       <c r="E6" s="8"/>
     </row>
     <row r="7" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -1130,7 +1181,7 @@
       <c r="C7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="16" t="s">
         <v>31</v>
       </c>
       <c r="E7" s="8"/>
@@ -1143,7 +1194,7 @@
       <c r="C8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="21" t="s">
         <v>16</v>
       </c>
       <c r="E8" s="8"/>
@@ -1156,7 +1207,7 @@
       <c r="C9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="16"/>
+      <c r="D9" s="21"/>
       <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -1167,7 +1218,7 @@
       <c r="C10" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="16" t="s">
         <v>21</v>
       </c>
       <c r="E10" s="8"/>
@@ -1180,7 +1231,7 @@
       <c r="C11" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="21" t="s">
         <v>24</v>
       </c>
       <c r="E11" s="8"/>
@@ -1193,7 +1244,7 @@
       <c r="C12" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="16"/>
+      <c r="D12" s="21"/>
       <c r="E12" s="8"/>
     </row>
     <row r="13" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -1204,7 +1255,7 @@
       <c r="C13" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="16"/>
+      <c r="D13" s="21"/>
       <c r="E13" s="8"/>
     </row>
     <row r="14" spans="1:5" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1215,7 +1266,7 @@
       <c r="C14" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="17"/>
+      <c r="D14" s="22"/>
       <c r="E14" s="8"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>